<commit_message>
fine tune gaming engineering courses
</commit_message>
<xml_diff>
--- a/api/python/TaiGerTranscriptAnalyzerJS/database/ComputerScience/CS_Course_database.xlsx
+++ b/api/python/TaiGerTranscriptAnalyzerJS/database/ComputerScience/CS_Course_database.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="214">
   <si>
     <t>所有科目</t>
   </si>
@@ -631,6 +631,30 @@
   </si>
   <si>
     <t xml:space="preserve">Signal Processing</t>
+  </si>
+  <si>
+    <t>社群遊戲</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social Gaming</t>
+  </si>
+  <si>
+    <t>實時電腦圖型</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real Time Computer Graphic</t>
+  </si>
+  <si>
+    <t>遊戲工程</t>
+  </si>
+  <si>
+    <t xml:space="preserve">games engineering</t>
+  </si>
+  <si>
+    <t>電腦遊戲</t>
+  </si>
+  <si>
+    <t xml:space="preserve">computer games</t>
   </si>
 </sst>
 </file>
@@ -4099,7 +4123,12 @@
       <c r="W103" s="9"/>
     </row>
     <row r="104" ht="16.199999999999999">
-      <c r="B104" s="3"/>
+      <c r="A104" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>207</v>
+      </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>
@@ -4120,8 +4149,13 @@
       <c r="V104" s="3"/>
       <c r="W104" s="9"/>
     </row>
-    <row r="105" ht="16.199999999999999">
-      <c r="B105" s="3"/>
+    <row r="105" ht="30">
+      <c r="A105" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>209</v>
+      </c>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
@@ -4143,7 +4177,12 @@
       <c r="W105" s="9"/>
     </row>
     <row r="106" ht="16.199999999999999">
-      <c r="B106" s="3"/>
+      <c r="A106" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>211</v>
+      </c>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
@@ -4165,7 +4204,12 @@
       <c r="W106" s="9"/>
     </row>
     <row r="107" ht="16.199999999999999">
-      <c r="B107" s="3"/>
+      <c r="A107" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>213</v>
+      </c>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>

</xml_diff>